<commit_message>
Se termino el desarrollo del servicio de carga de horarios
Se termino el desarrollo y testeo del servicio para importar horarios.
</commit_message>
<xml_diff>
--- a/src/test/resources/Import Sample Test 2.xlsx
+++ b/src/test/resources/Import Sample Test 2.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Victor\Desktop\TIP\backend-tip\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9E52D4-A0EF-4054-B926-76B001D5A7FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F048AAF-4F2C-4494-BC12-312BA2EB51DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="1020" windowWidth="15375" windowHeight="8325" xr2:uid="{5C8D9C40-CB1B-43C9-A79C-5280D339B0FD}"/>
+    <workbookView xWindow="1920" yWindow="1710" windowWidth="15375" windowHeight="8325" xr2:uid="{5C8D9C40-CB1B-43C9-A79C-5280D339B0FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Importar" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -451,7 +451,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>